<commit_message>
solarbr changes to templates and code update
</commit_message>
<xml_diff>
--- a/Projects/SOLARBR/Data/Score Template.xlsx
+++ b/Projects/SOLARBR/Data/Score Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="DROGARIA" sheetId="1" state="visible" r:id="rId2"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="36">
   <si>
     <t xml:space="preserve">Kpi</t>
   </si>
@@ -89,7 +89,7 @@
     <t xml:space="preserve">SOVI CERVEJA GELADO</t>
   </si>
   <si>
-    <t xml:space="preserve">SOVI RET Gelado KO FAM</t>
+    <t xml:space="preserve">SOVI RET GELADO KO FAM</t>
   </si>
   <si>
     <t xml:space="preserve">SOVI FANTA LARANJA</t>
@@ -98,13 +98,10 @@
     <t xml:space="preserve">SOVI SSD Balcão Refrigerado KO</t>
   </si>
   <si>
-    <t xml:space="preserve">SOVI SUCO </t>
+    <t xml:space="preserve">SOVI SUCO</t>
   </si>
   <si>
     <t xml:space="preserve">SOVI SSD SABORES KO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SOVI SSD gelado KO</t>
   </si>
   <si>
     <t xml:space="preserve">SOVI RET KO FAM</t>
@@ -113,19 +110,10 @@
     <t xml:space="preserve">SOVI STILL Balcão Refrigerado</t>
   </si>
   <si>
-    <t xml:space="preserve">SOVI RET GELADO KO FAM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SOVI SUCO</t>
-  </si>
-  <si>
     <t xml:space="preserve">SOVI SS SSD KO</t>
   </si>
   <si>
     <t xml:space="preserve">SOVI ADES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SOVI ENERGÉTICO</t>
   </si>
   <si>
     <t xml:space="preserve">SOVI SSD LOW CALS</t>
@@ -141,6 +129,9 @@
   </si>
   <si>
     <t xml:space="preserve">SOVI SSD KO SEÇÃO DE BEBIDAS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOVI ENERGÉTICO</t>
   </si>
   <si>
     <t xml:space="preserve">SOVI CCTM</t>
@@ -220,7 +211,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -239,13 +230,26 @@
         <bgColor rgb="FF969696"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFCCFFCC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
   </borders>
@@ -278,7 +282,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -371,6 +375,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="167" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -425,7 +433,7 @@
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FFDDDDDD"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -471,24 +479,24 @@
   <dimension ref="A1:N31"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E30" activeCellId="1" sqref="E32 E30"/>
+      <selection pane="topLeft" activeCell="A26" activeCellId="1" sqref="A38:A41 A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.3846153846154"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.8137651821862"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.1417004048583"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="13.0688259109312"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.3522267206478"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="13.2834008097166"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.5668016194332"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.1417004048583"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.4939271255061"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.7085020242915"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="4.39271255060729"/>
     <col collapsed="false" hidden="false" max="12" min="11" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="13" min="13" style="0" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="13.0688259109312"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="13.2834008097166"/>
     <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -1003,12 +1011,12 @@
   <dimension ref="A1:S65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K54" activeCellId="1" sqref="E32 K54"/>
+      <selection pane="topLeft" activeCell="K54" activeCellId="1" sqref="A38:A41 K54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="35.0283400809717"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="35.4574898785425"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.1417004048583"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.63967611336032"/>
@@ -1016,12 +1024,12 @@
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.7085020242915"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.9230769230769"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="4.39271255060729"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="13" min="13" style="0" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="13.0688259109312"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="13.2834008097166"/>
     <col collapsed="false" hidden="false" max="15" min="15" style="0" width="3.64372469635628"/>
     <col collapsed="false" hidden="false" max="16" min="16" style="0" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="17" min="17" style="0" width="8.1417004048583"/>
@@ -1177,11 +1185,11 @@
         <v>3.5</v>
       </c>
       <c r="I6" s="3"/>
-      <c r="J6" s="24"/>
+      <c r="J6" s="25"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B7" s="5" t="n">
         <v>0</v>
@@ -1198,7 +1206,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B8" s="5" t="n">
         <v>0.15</v>
@@ -1215,7 +1223,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B9" s="5" t="n">
         <v>0.2</v>
@@ -1232,7 +1240,7 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B10" s="5" t="n">
         <v>0.25</v>
@@ -1249,7 +1257,7 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B11" s="5" t="n">
         <v>0.3</v>
@@ -1504,7 +1512,7 @@
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B26" s="5" t="n">
         <v>0</v>
@@ -1521,7 +1529,7 @@
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B27" s="5" t="n">
         <v>0.3</v>
@@ -1546,7 +1554,7 @@
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B28" s="5" t="n">
         <v>0.35</v>
@@ -1571,7 +1579,7 @@
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B29" s="5" t="n">
         <v>0.4</v>
@@ -1586,7 +1594,7 @@
         <v>1</v>
       </c>
       <c r="I29" s="3"/>
-      <c r="J29" s="24"/>
+      <c r="J29" s="25"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
@@ -1845,7 +1853,7 @@
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B45" s="5" t="n">
         <v>0</v>
@@ -1862,7 +1870,7 @@
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B46" s="5" t="n">
         <v>0.15</v>
@@ -1879,7 +1887,7 @@
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B47" s="5" t="n">
         <v>0.2</v>
@@ -1896,7 +1904,7 @@
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B48" s="5" t="n">
         <v>0.25</v>
@@ -1913,7 +1921,7 @@
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B49" s="5" t="n">
         <v>0.3</v>
@@ -2043,7 +2051,7 @@
       <c r="D56" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="E56" s="25" t="n">
+      <c r="E56" s="26" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2076,12 +2084,12 @@
   <dimension ref="A1:S59"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E59" activeCellId="1" sqref="E32 E59"/>
+      <selection pane="topLeft" activeCell="E59" activeCellId="1" sqref="A38:A41 E59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.4210526315789"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.0647773279352"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.1417004048583"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.63967611336032"/>
@@ -2089,7 +2097,7 @@
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.7085020242915"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.9230769230769"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="4.39271255060729"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="7.49797570850202"/>
@@ -2262,7 +2270,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B7" s="5" t="n">
         <v>0</v>
@@ -2281,7 +2289,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B8" s="5" t="n">
         <v>0.15</v>
@@ -2298,7 +2306,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B9" s="5" t="n">
         <v>0.2</v>
@@ -2315,7 +2323,7 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B10" s="5" t="n">
         <v>0.25</v>
@@ -2332,7 +2340,7 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B11" s="5" t="n">
         <v>0.3</v>
@@ -2587,7 +2595,7 @@
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B26" s="5" t="n">
         <v>0</v>
@@ -2604,7 +2612,7 @@
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B27" s="5" t="n">
         <v>0.3</v>
@@ -2621,7 +2629,7 @@
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B28" s="5" t="n">
         <v>0.35</v>
@@ -2638,7 +2646,7 @@
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B29" s="5" t="n">
         <v>0.4</v>
@@ -2910,7 +2918,7 @@
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B45" s="5" t="n">
         <v>0</v>
@@ -2927,7 +2935,7 @@
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B46" s="5" t="n">
         <v>0.15</v>
@@ -2944,7 +2952,7 @@
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B47" s="5" t="n">
         <v>0.2</v>
@@ -2961,7 +2969,7 @@
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B48" s="5" t="n">
         <v>0.25</v>
@@ -2978,7 +2986,7 @@
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B49" s="5" t="n">
         <v>0.3</v>
@@ -3108,7 +3116,7 @@
       <c r="D56" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="E56" s="23" t="n">
+      <c r="E56" s="24" t="n">
         <v>1</v>
       </c>
     </row>
@@ -3139,12 +3147,12 @@
   <dimension ref="A1:S65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E6" activeCellId="1" sqref="E32 E6"/>
+      <selection pane="topLeft" activeCell="E6" activeCellId="1" sqref="A38:A41 E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.5627530364372"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.9919028340081"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="22" width="8.1417004048583"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="6.63967611336032"/>
@@ -3152,7 +3160,7 @@
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="22" width="8.1417004048583"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.7085020242915"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.9230769230769"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="4.39271255060729"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="22" width="8.1417004048583"/>
@@ -3505,7 +3513,7 @@
       <c r="D16" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="E16" s="26" t="n">
+      <c r="E16" s="27" t="n">
         <v>0</v>
       </c>
       <c r="G16" s="0"/>
@@ -3547,7 +3555,7 @@
       <c r="D18" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="E18" s="26" t="n">
+      <c r="E18" s="27" t="n">
         <v>1</v>
       </c>
       <c r="G18" s="0"/>
@@ -3699,7 +3707,7 @@
       <c r="D25" s="5" t="n">
         <v>0.5</v>
       </c>
-      <c r="E25" s="27" t="n">
+      <c r="E25" s="28" t="n">
         <v>0.5</v>
       </c>
       <c r="G25" s="0"/>
@@ -3721,7 +3729,7 @@
       <c r="D26" s="5" t="n">
         <v>0.75</v>
       </c>
-      <c r="E26" s="27" t="n">
+      <c r="E26" s="28" t="n">
         <v>0.75</v>
       </c>
       <c r="G26" s="0"/>
@@ -3743,7 +3751,7 @@
       <c r="D27" s="5" t="n">
         <v>0.95</v>
       </c>
-      <c r="E27" s="27" t="n">
+      <c r="E27" s="28" t="n">
         <v>0.95</v>
       </c>
       <c r="G27" s="0"/>
@@ -3807,7 +3815,7 @@
       <c r="D30" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="E30" s="23" t="n">
+      <c r="E30" s="24" t="n">
         <v>1</v>
       </c>
       <c r="G30" s="0"/>
@@ -3818,7 +3826,7 @@
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B31" s="5" t="n">
         <v>0</v>
@@ -3840,7 +3848,7 @@
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B32" s="5" t="n">
         <v>0.15</v>
@@ -3862,7 +3870,7 @@
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B33" s="5" t="n">
         <v>0.2</v>
@@ -4031,7 +4039,7 @@
       <c r="D41" s="5" t="n">
         <v>0.75</v>
       </c>
-      <c r="E41" s="27" t="n">
+      <c r="E41" s="28" t="n">
         <v>1.13</v>
       </c>
     </row>
@@ -4048,7 +4056,7 @@
       <c r="D42" s="5" t="n">
         <v>0.95</v>
       </c>
-      <c r="E42" s="27" t="n">
+      <c r="E42" s="28" t="n">
         <v>1.43</v>
       </c>
     </row>
@@ -4071,7 +4079,7 @@
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B44" s="5" t="n">
         <v>0</v>
@@ -4088,7 +4096,7 @@
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B45" s="5" t="n">
         <v>0.25</v>
@@ -4105,7 +4113,7 @@
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B46" s="5" t="n">
         <v>0.3</v>
@@ -4122,7 +4130,7 @@
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B47" s="5" t="n">
         <v>0.35</v>
@@ -4133,13 +4141,13 @@
       <c r="D47" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="E47" s="23" t="n">
+      <c r="E47" s="24" t="n">
         <v>0.5</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B48" s="5" t="n">
         <v>0</v>
@@ -4156,7 +4164,7 @@
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B49" s="5" t="n">
         <v>0.06</v>
@@ -4173,7 +4181,7 @@
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B50" s="5" t="n">
         <v>0.07</v>
@@ -4190,7 +4198,7 @@
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B51" s="5" t="n">
         <v>0.085</v>
@@ -4207,7 +4215,7 @@
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B52" s="5" t="n">
         <v>0.1</v>
@@ -4309,7 +4317,7 @@
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B58" s="5" t="n">
         <v>0</v>
@@ -4326,7 +4334,7 @@
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B59" s="5" t="n">
         <v>0.06</v>
@@ -4343,7 +4351,7 @@
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B60" s="5" t="n">
         <v>0.07</v>
@@ -4360,7 +4368,7 @@
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B61" s="5" t="n">
         <v>0.085</v>
@@ -4377,7 +4385,7 @@
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B62" s="5" t="n">
         <v>0.1</v>
@@ -4394,7 +4402,7 @@
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B63" s="5" t="n">
         <v>0</v>
@@ -4411,7 +4419,7 @@
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B64" s="5" t="n">
         <v>0.6</v>
@@ -4422,13 +4430,13 @@
       <c r="D64" s="5" t="n">
         <v>0.5</v>
       </c>
-      <c r="E64" s="27" t="n">
+      <c r="E64" s="28" t="n">
         <v>0.5</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B65" s="5" t="n">
         <v>0.66</v>
@@ -4439,13 +4447,13 @@
       <c r="D65" s="5" t="n">
         <v>0.75</v>
       </c>
-      <c r="E65" s="27" t="n">
+      <c r="E65" s="28" t="n">
         <v>0.75</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B66" s="5" t="n">
         <v>0.7</v>
@@ -4456,13 +4464,13 @@
       <c r="D66" s="5" t="n">
         <v>0.95</v>
       </c>
-      <c r="E66" s="27" t="n">
+      <c r="E66" s="28" t="n">
         <v>0.95</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B67" s="5" t="n">
         <v>0.75</v>
@@ -4505,13 +4513,13 @@
   </sheetPr>
   <dimension ref="A1:X65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A52" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A81" activeCellId="1" sqref="E32 A81"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A16" activeCellId="1" sqref="A38:A41 A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.1740890688259"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.4939271255061"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="22" width="8.1417004048583"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.63967611336032"/>
@@ -4519,7 +4527,7 @@
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="22" width="8.1417004048583"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.7085020242915"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.9230769230769"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="4.39271255060729"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="22" width="8.1417004048583"/>
@@ -4849,7 +4857,7 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B12" s="5" t="n">
         <v>0</v>
@@ -4879,7 +4887,7 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B13" s="5" t="n">
         <v>0.25</v>
@@ -4909,7 +4917,7 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B14" s="5" t="n">
         <v>0.3</v>
@@ -4939,7 +4947,7 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B15" s="5" t="n">
         <v>0.35</v>
@@ -4985,7 +4993,7 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="B17" s="5" t="n">
         <v>0</v>
@@ -5018,7 +5026,7 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="B18" s="5" t="n">
         <v>0.05</v>
@@ -5048,7 +5056,7 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="B19" s="5" t="n">
         <v>0.15</v>
@@ -5101,7 +5109,7 @@
       <c r="D21" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="E21" s="23" t="n">
+      <c r="E21" s="24" t="n">
         <v>1</v>
       </c>
       <c r="F21" s="5"/>
@@ -5610,7 +5618,7 @@
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B39" s="5" t="n">
         <v>0</v>
@@ -5639,7 +5647,7 @@
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B40" s="5" t="n">
         <v>0.25</v>
@@ -5668,7 +5676,7 @@
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B41" s="5" t="n">
         <v>0.3</v>
@@ -5696,7 +5704,7 @@
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B42" s="5" t="n">
         <v>0.35</v>
@@ -5707,7 +5715,7 @@
       <c r="D42" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="E42" s="23" t="n">
+      <c r="E42" s="24" t="n">
         <v>0.5</v>
       </c>
       <c r="G42" s="0"/>
@@ -5755,7 +5763,7 @@
       <c r="D44" s="5" t="n">
         <v>0.5</v>
       </c>
-      <c r="E44" s="27" t="n">
+      <c r="E44" s="28" t="n">
         <v>0.5</v>
       </c>
       <c r="G44" s="0"/>
@@ -5775,7 +5783,7 @@
       <c r="D45" s="5" t="n">
         <v>0.75</v>
       </c>
-      <c r="E45" s="27" t="n">
+      <c r="E45" s="28" t="n">
         <v>0.75</v>
       </c>
       <c r="G45" s="0"/>
@@ -5795,7 +5803,7 @@
       <c r="D46" s="5" t="n">
         <v>0.95</v>
       </c>
-      <c r="E46" s="27" t="n">
+      <c r="E46" s="28" t="n">
         <v>0.95</v>
       </c>
       <c r="G46" s="0"/>
@@ -5824,7 +5832,7 @@
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B48" s="5" t="n">
         <v>0</v>
@@ -5844,7 +5852,7 @@
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B49" s="5" t="n">
         <v>0.15</v>
@@ -5855,7 +5863,7 @@
       <c r="D49" s="5" t="n">
         <v>0.5</v>
       </c>
-      <c r="E49" s="27" t="n">
+      <c r="E49" s="28" t="n">
         <v>0.5</v>
       </c>
       <c r="G49" s="0"/>
@@ -5864,7 +5872,7 @@
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B50" s="5" t="n">
         <v>0.2</v>
@@ -5875,7 +5883,7 @@
       <c r="D50" s="5" t="n">
         <v>0.75</v>
       </c>
-      <c r="E50" s="27" t="n">
+      <c r="E50" s="28" t="n">
         <v>0.75</v>
       </c>
       <c r="G50" s="0"/>
@@ -5884,7 +5892,7 @@
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B51" s="5" t="n">
         <v>0.25</v>
@@ -5895,13 +5903,13 @@
       <c r="D51" s="5" t="n">
         <v>0.95</v>
       </c>
-      <c r="E51" s="27" t="n">
+      <c r="E51" s="28" t="n">
         <v>0.95</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B52" s="5" t="n">
         <v>0.3</v>
@@ -5918,7 +5926,7 @@
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B53" s="5" t="n">
         <v>0</v>
@@ -5935,7 +5943,7 @@
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B54" s="5" t="n">
         <v>0.25</v>
@@ -5952,7 +5960,7 @@
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B55" s="5" t="n">
         <v>0.3</v>
@@ -5969,7 +5977,7 @@
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B56" s="5" t="n">
         <v>0.35</v>
@@ -5986,7 +5994,7 @@
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B57" s="5" t="n">
         <v>0</v>
@@ -6003,7 +6011,7 @@
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B58" s="5" t="n">
         <v>0.2</v>
@@ -6020,7 +6028,7 @@
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B59" s="5" t="n">
         <v>0.3</v>
@@ -6037,7 +6045,7 @@
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B60" s="5" t="n">
         <v>0</v>
@@ -6054,7 +6062,7 @@
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B61" s="5" t="n">
         <v>0.6</v>
@@ -6071,7 +6079,7 @@
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B62" s="5" t="n">
         <v>0.66</v>
@@ -6088,7 +6096,7 @@
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B63" s="5" t="n">
         <v>0.7</v>
@@ -6105,7 +6113,7 @@
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B64" s="5" t="n">
         <v>0.75</v>
@@ -6235,7 +6243,7 @@
       <c r="D71" s="5" t="n">
         <v>0.5</v>
       </c>
-      <c r="E71" s="27" t="n">
+      <c r="E71" s="28" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -6252,7 +6260,7 @@
       <c r="D72" s="5" t="n">
         <v>0.75</v>
       </c>
-      <c r="E72" s="27" t="n">
+      <c r="E72" s="28" t="n">
         <v>0.75</v>
       </c>
     </row>
@@ -6269,7 +6277,7 @@
       <c r="D73" s="5" t="n">
         <v>0.95</v>
       </c>
-      <c r="E73" s="27" t="n">
+      <c r="E73" s="28" t="n">
         <v>0.95</v>
       </c>
     </row>
@@ -6292,7 +6300,7 @@
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B75" s="5" t="n">
         <v>0</v>
@@ -6309,7 +6317,7 @@
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B76" s="5" t="n">
         <v>0.2</v>
@@ -6326,7 +6334,7 @@
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B77" s="5" t="n">
         <v>0.3</v>
@@ -6369,12 +6377,12 @@
   <dimension ref="A1:N65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I49" activeCellId="1" sqref="E32 I49"/>
+      <selection pane="topLeft" activeCell="I49" activeCellId="1" sqref="A38:A41 I49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.7085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.1376518218623"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.63967611336032"/>
@@ -6382,7 +6390,7 @@
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.1012145748988"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.3157894736842"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="4.39271255060729"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="7.49797570850202"/>
@@ -6393,7 +6401,7 @@
     <col collapsed="false" hidden="false" max="17" min="17" style="0" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="18" min="18" style="0" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="19" min="19" style="0" width="6.63967611336032"/>
-    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="19.8178137651822"/>
+    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6519,7 +6527,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B7" s="5" t="n">
         <v>0</v>
@@ -6536,7 +6544,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B8" s="5" t="n">
         <v>0.6</v>
@@ -6553,7 +6561,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B9" s="5" t="n">
         <v>0.66</v>
@@ -6570,7 +6578,7 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B10" s="5" t="n">
         <v>0.7</v>
@@ -6587,7 +6595,7 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B11" s="5" t="n">
         <v>0.75</v>
@@ -6604,7 +6612,7 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B12" s="5" t="n">
         <v>0</v>
@@ -6621,7 +6629,7 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B13" s="5" t="n">
         <v>0.05</v>
@@ -6638,7 +6646,7 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B14" s="5" t="n">
         <v>0.15</v>
@@ -6655,7 +6663,7 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B15" s="5" t="n">
         <v>0</v>
@@ -6672,7 +6680,7 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B16" s="5" t="n">
         <v>0.3</v>
@@ -6689,7 +6697,7 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B17" s="5" t="n">
         <v>0.33</v>
@@ -6706,7 +6714,7 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B18" s="5" t="n">
         <v>0.35</v>
@@ -6730,7 +6738,7 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B19" s="5" t="n">
         <v>0.38</v>
@@ -6872,7 +6880,7 @@
       <c r="D26" s="5" t="n">
         <v>0.5</v>
       </c>
-      <c r="E26" s="27" t="n">
+      <c r="E26" s="28" t="n">
         <v>0.25</v>
       </c>
     </row>
@@ -6895,7 +6903,7 @@
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B28" s="5" t="n">
         <v>0</v>
@@ -6912,7 +6920,7 @@
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B29" s="5" t="n">
         <v>0.2</v>
@@ -6929,7 +6937,7 @@
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B30" s="5" t="n">
         <v>0.33</v>
@@ -7099,7 +7107,7 @@
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B40" s="5" t="n">
         <v>0</v>
@@ -7116,7 +7124,7 @@
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B41" s="5" t="n">
         <v>0.6</v>
@@ -7133,7 +7141,7 @@
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B42" s="5" t="n">
         <v>0.66</v>
@@ -7150,7 +7158,7 @@
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B43" s="5" t="n">
         <v>0.7</v>
@@ -7167,7 +7175,7 @@
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B44" s="5" t="n">
         <v>0.75</v>
@@ -7184,7 +7192,7 @@
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B45" s="5" t="n">
         <v>0</v>
@@ -7201,7 +7209,7 @@
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B46" s="5" t="n">
         <v>0.25</v>
@@ -7218,7 +7226,7 @@
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B47" s="5" t="n">
         <v>0.3</v>
@@ -7235,7 +7243,7 @@
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B48" s="5" t="n">
         <v>0.35</v>
@@ -7278,19 +7286,19 @@
   <dimension ref="A1:E42"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E42" activeCellId="1" sqref="E32 E42"/>
+      <selection pane="topLeft" activeCell="E42" activeCellId="1" sqref="A38:A41 E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.7813765182186"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="18.9595141700405"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.995951417004"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="19.3886639676113"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.3562753036437"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.1417004048583"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.7085020242915"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.9230769230769"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="4.39271255060729"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.1417004048583"/>
@@ -8011,12 +8019,12 @@
   <dimension ref="A1:O18"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E18" activeCellId="1" sqref="E32 E18"/>
+      <selection pane="topLeft" activeCell="E18" activeCellId="1" sqref="A38:A41 E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.7085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="35.1336032388664"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="13.9271255060729"/>
@@ -8024,7 +8032,7 @@
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.7085020242915"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.9230769230769"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="4.39271255060729"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="7.49797570850202"/>
@@ -8335,20 +8343,20 @@
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E18" activeCellId="1" sqref="E32 E18"/>
+      <selection pane="topLeft" activeCell="E18" activeCellId="1" sqref="A38:A41 E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.995951417004"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.3522267206478"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.2105263157895"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.5668016194332"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="12.5344129554656"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="12.748987854251"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.7085020242915"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.9230769230769"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="4.39271255060729"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="7.49797570850202"/>
@@ -8657,28 +8665,28 @@
   </sheetPr>
   <dimension ref="A1:S32"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E32" activeCellId="0" sqref="E32"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E32" activeCellId="1" sqref="A38:A41 E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.5303643724696"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.8906882591093"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.246963562753"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.0647773279352"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.1012145748988"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.4615384615385"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="14.0323886639676"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.7813765182186"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.7085020242915"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.9230769230769"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="4.39271255060729"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.1417004048583"/>
     <col collapsed="false" hidden="false" max="13" min="13" style="0" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="0" width="6.63967611336032"/>
     <col collapsed="false" hidden="false" max="18" min="15" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="13.0688259109312"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="13.2834008097166"/>
     <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -9219,12 +9227,12 @@
   <dimension ref="A1:S32"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E32" activeCellId="0" sqref="E32"/>
+      <selection pane="topLeft" activeCell="E32" activeCellId="1" sqref="A38:A41 E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="54.417004048583"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="55.4858299595142"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.46153846153846"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.78542510121457"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="18" width="6.63967611336032"/>
@@ -9232,14 +9240,14 @@
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.7085020242915"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.9230769230769"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="4.39271255060729"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.1417004048583"/>
     <col collapsed="false" hidden="false" max="13" min="13" style="0" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="0" width="6.63967611336032"/>
     <col collapsed="false" hidden="false" max="18" min="15" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="13.0688259109312"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="13.2834008097166"/>
     <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -9787,20 +9795,20 @@
   <dimension ref="A1:S65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E29" activeCellId="1" sqref="E32 E29"/>
+      <selection pane="topLeft" activeCell="E29" activeCellId="1" sqref="A38:A41 E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.17004048583"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.7044534412955"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.1417004048583"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.1781376518219"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="3.64372469635628"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.1417004048583"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.7085020242915"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.9230769230769"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="4.39271255060729"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="7.49797570850202"/>
@@ -10324,12 +10332,12 @@
   <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E29" activeCellId="1" sqref="E32 E29"/>
+      <selection pane="topLeft" activeCell="E29" activeCellId="1" sqref="A38:A41 E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.8866396761134"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.4210526315789"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.1417004048583"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.67611336032389"/>
@@ -10337,7 +10345,7 @@
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.1417004048583"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.7085020242915"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.9230769230769"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="4.39271255060729"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="7.49797570850202"/>
@@ -10823,13 +10831,13 @@
   </sheetPr>
   <dimension ref="A1:S65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E63" activeCellId="1" sqref="E32 E63"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A38" activeCellId="0" sqref="A38:A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.6720647773279"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.1012145748988"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="22" width="8.1417004048583"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="10" width="6.63967611336032"/>
@@ -10837,7 +10845,7 @@
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="22" width="8.1417004048583"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="10" width="19.7085020242915"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="10" width="19.9230769230769"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="4.39271255060729"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="22" width="8.1417004048583"/>
@@ -11016,7 +11024,7 @@
       <c r="S6" s="16"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="23" t="s">
         <v>18</v>
       </c>
       <c r="B7" s="5" t="n">
@@ -11043,7 +11051,7 @@
       <c r="S7" s="16"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="23" t="s">
         <v>18</v>
       </c>
       <c r="B8" s="5" t="n">
@@ -11070,7 +11078,7 @@
       <c r="S8" s="16"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="23" t="s">
         <v>18</v>
       </c>
       <c r="B9" s="5" t="n">
@@ -11094,7 +11102,7 @@
       <c r="S9" s="0"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="23" t="s">
         <v>18</v>
       </c>
       <c r="B10" s="5" t="n">
@@ -11117,7 +11125,7 @@
       <c r="S10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="23" t="s">
         <v>18</v>
       </c>
       <c r="B11" s="5" t="n">
@@ -11268,7 +11276,7 @@
       <c r="D17" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="E17" s="23" t="n">
+      <c r="E17" s="24" t="n">
         <v>1</v>
       </c>
       <c r="G17" s="0"/>
@@ -11752,8 +11760,8 @@
       <c r="S36" s="0"/>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
-        <v>23</v>
+      <c r="A37" s="7" t="s">
+        <v>13</v>
       </c>
       <c r="B37" s="5" t="n">
         <v>0</v>
@@ -11775,8 +11783,8 @@
       <c r="S37" s="0"/>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
-        <v>23</v>
+      <c r="A38" s="7" t="s">
+        <v>13</v>
       </c>
       <c r="B38" s="5" t="n">
         <v>0.6</v>
@@ -11792,8 +11800,8 @@
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="s">
-        <v>23</v>
+      <c r="A39" s="7" t="s">
+        <v>13</v>
       </c>
       <c r="B39" s="5" t="n">
         <v>0.66</v>
@@ -11809,8 +11817,8 @@
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="s">
-        <v>23</v>
+      <c r="A40" s="7" t="s">
+        <v>13</v>
       </c>
       <c r="B40" s="5" t="n">
         <v>0.7</v>
@@ -11826,8 +11834,8 @@
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="s">
-        <v>23</v>
+      <c r="A41" s="7" t="s">
+        <v>13</v>
       </c>
       <c r="B41" s="5" t="n">
         <v>0.75</v>
@@ -11895,7 +11903,7 @@
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B45" s="5" t="n">
         <v>0</v>
@@ -11912,7 +11920,7 @@
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B46" s="5" t="n">
         <v>0.06</v>
@@ -11929,7 +11937,7 @@
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B47" s="5" t="n">
         <v>0.07</v>
@@ -11946,7 +11954,7 @@
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B48" s="5" t="n">
         <v>0.085</v>
@@ -11963,7 +11971,7 @@
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B49" s="5" t="n">
         <v>0.1</v>
@@ -12065,7 +12073,7 @@
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B55" s="5" t="n">
         <v>0</v>
@@ -12082,7 +12090,7 @@
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B56" s="5" t="n">
         <v>0.3</v>
@@ -12099,7 +12107,7 @@
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B57" s="5" t="n">
         <v>0.35</v>
@@ -12116,7 +12124,7 @@
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B58" s="5" t="n">
         <v>0.4</v>
@@ -12133,7 +12141,7 @@
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B59" s="5" t="n">
         <v>0.45</v>
@@ -12149,10 +12157,20 @@
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="3" t="s">
+      <c r="B63" s="0"/>
+      <c r="D63" s="0"/>
+      <c r="G63" s="0"/>
+      <c r="I63" s="0"/>
+      <c r="L63" s="0"/>
+      <c r="N63" s="0"/>
+      <c r="Q63" s="0"/>
+      <c r="S63" s="0"/>
+    </row>
+    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E63" s="0" t="n">
+      <c r="E72" s="0" t="n">
         <v>25.5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
score template update - fixed lower to upper issue
</commit_message>
<xml_diff>
--- a/Projects/SOLARBR/Data/Score Template.xlsx
+++ b/Projects/SOLARBR/Data/Score Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="8"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="DROGARIA" sheetId="1" state="visible" r:id="rId2"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="34">
   <si>
     <t xml:space="preserve">Kpi</t>
   </si>
@@ -95,9 +95,6 @@
     <t xml:space="preserve">SOVI FANTA LARANJA</t>
   </si>
   <si>
-    <t xml:space="preserve">SOVI SSD Balcão Refrigerado KO</t>
-  </si>
-  <si>
     <t xml:space="preserve">SOVI SUCO</t>
   </si>
   <si>
@@ -105,9 +102,6 @@
   </si>
   <si>
     <t xml:space="preserve">SOVI RET KO FAM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SOVI STILL Balcão Refrigerado</t>
   </si>
   <si>
     <t xml:space="preserve">SOVI SS SSD KO</t>
@@ -282,7 +276,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -383,6 +377,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="167" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -479,24 +477,24 @@
   <dimension ref="A1:N31"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A26" activeCellId="1" sqref="A38:A41 A26"/>
+      <selection pane="topLeft" activeCell="A26" activeCellId="0" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.8137651821862"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.0283400809717"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.1417004048583"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="13.2834008097166"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.5668016194332"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="13.3886639676113"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.6720647773279"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.1417004048583"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.7085020242915"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.8178137651822"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="4.39271255060729"/>
     <col collapsed="false" hidden="false" max="12" min="11" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="13" min="13" style="0" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="13.2834008097166"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -1011,12 +1009,12 @@
   <dimension ref="A1:S65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K54" activeCellId="1" sqref="A38:A41 K54"/>
+      <selection pane="topLeft" activeCell="K54" activeCellId="0" sqref="K54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="35.4574898785425"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="35.6720647773279"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.1417004048583"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.63967611336032"/>
@@ -1024,12 +1022,12 @@
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.9230769230769"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="20.0323886639676"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="4.39271255060729"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="13" min="13" style="0" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="13.2834008097166"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="15" min="15" style="0" width="3.64372469635628"/>
     <col collapsed="false" hidden="false" max="16" min="16" style="0" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="17" min="17" style="0" width="8.1417004048583"/>
@@ -1185,7 +1183,7 @@
         <v>3.5</v>
       </c>
       <c r="I6" s="3"/>
-      <c r="J6" s="25"/>
+      <c r="J6" s="26"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
@@ -1512,7 +1510,7 @@
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B26" s="5" t="n">
         <v>0</v>
@@ -1529,7 +1527,7 @@
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B27" s="5" t="n">
         <v>0.3</v>
@@ -1554,7 +1552,7 @@
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B28" s="5" t="n">
         <v>0.35</v>
@@ -1579,7 +1577,7 @@
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B29" s="5" t="n">
         <v>0.4</v>
@@ -1594,7 +1592,7 @@
         <v>1</v>
       </c>
       <c r="I29" s="3"/>
-      <c r="J29" s="25"/>
+      <c r="J29" s="26"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
@@ -1853,7 +1851,7 @@
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B45" s="5" t="n">
         <v>0</v>
@@ -1870,7 +1868,7 @@
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B46" s="5" t="n">
         <v>0.15</v>
@@ -1887,7 +1885,7 @@
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B47" s="5" t="n">
         <v>0.2</v>
@@ -1904,7 +1902,7 @@
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B48" s="5" t="n">
         <v>0.25</v>
@@ -1921,7 +1919,7 @@
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B49" s="5" t="n">
         <v>0.3</v>
@@ -2051,7 +2049,7 @@
       <c r="D56" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="E56" s="26" t="n">
+      <c r="E56" s="27" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2084,12 +2082,12 @@
   <dimension ref="A1:S59"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E59" activeCellId="1" sqref="A38:A41 E59"/>
+      <selection pane="topLeft" activeCell="E59" activeCellId="0" sqref="E59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.0647773279352"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.3846153846154"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.1417004048583"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.63967611336032"/>
@@ -2097,7 +2095,7 @@
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.9230769230769"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="20.0323886639676"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="4.39271255060729"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="7.49797570850202"/>
@@ -2595,7 +2593,7 @@
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B26" s="5" t="n">
         <v>0</v>
@@ -2612,7 +2610,7 @@
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B27" s="5" t="n">
         <v>0.3</v>
@@ -2629,7 +2627,7 @@
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B28" s="5" t="n">
         <v>0.35</v>
@@ -2646,7 +2644,7 @@
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B29" s="5" t="n">
         <v>0.4</v>
@@ -2918,7 +2916,7 @@
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B45" s="5" t="n">
         <v>0</v>
@@ -2935,7 +2933,7 @@
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B46" s="5" t="n">
         <v>0.15</v>
@@ -2952,7 +2950,7 @@
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B47" s="5" t="n">
         <v>0.2</v>
@@ -2969,7 +2967,7 @@
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B48" s="5" t="n">
         <v>0.25</v>
@@ -2986,7 +2984,7 @@
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B49" s="5" t="n">
         <v>0.3</v>
@@ -3147,12 +3145,12 @@
   <dimension ref="A1:S65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E6" activeCellId="1" sqref="A38:A41 E6"/>
+      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.9919028340081"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.2064777327935"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="22" width="8.1417004048583"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="6.63967611336032"/>
@@ -3160,7 +3158,7 @@
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="22" width="8.1417004048583"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.9230769230769"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="20.0323886639676"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="4.39271255060729"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="22" width="8.1417004048583"/>
@@ -3513,7 +3511,7 @@
       <c r="D16" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="E16" s="27" t="n">
+      <c r="E16" s="28" t="n">
         <v>0</v>
       </c>
       <c r="G16" s="0"/>
@@ -3555,7 +3553,7 @@
       <c r="D18" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="E18" s="27" t="n">
+      <c r="E18" s="28" t="n">
         <v>1</v>
       </c>
       <c r="G18" s="0"/>
@@ -3707,7 +3705,7 @@
       <c r="D25" s="5" t="n">
         <v>0.5</v>
       </c>
-      <c r="E25" s="28" t="n">
+      <c r="E25" s="29" t="n">
         <v>0.5</v>
       </c>
       <c r="G25" s="0"/>
@@ -3729,7 +3727,7 @@
       <c r="D26" s="5" t="n">
         <v>0.75</v>
       </c>
-      <c r="E26" s="28" t="n">
+      <c r="E26" s="29" t="n">
         <v>0.75</v>
       </c>
       <c r="G26" s="0"/>
@@ -3751,7 +3749,7 @@
       <c r="D27" s="5" t="n">
         <v>0.95</v>
       </c>
-      <c r="E27" s="28" t="n">
+      <c r="E27" s="29" t="n">
         <v>0.95</v>
       </c>
       <c r="G27" s="0"/>
@@ -3826,7 +3824,7 @@
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B31" s="5" t="n">
         <v>0</v>
@@ -3848,7 +3846,7 @@
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B32" s="5" t="n">
         <v>0.15</v>
@@ -3870,7 +3868,7 @@
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B33" s="5" t="n">
         <v>0.2</v>
@@ -3892,7 +3890,7 @@
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B34" s="5" t="n">
         <v>0</v>
@@ -3914,7 +3912,7 @@
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B35" s="5" t="n">
         <v>0.6</v>
@@ -3934,7 +3932,7 @@
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B36" s="5" t="n">
         <v>0.66</v>
@@ -3954,7 +3952,7 @@
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B37" s="5" t="n">
         <v>0.7</v>
@@ -3974,7 +3972,7 @@
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B38" s="5" t="n">
         <v>0.75</v>
@@ -4039,7 +4037,7 @@
       <c r="D41" s="5" t="n">
         <v>0.75</v>
       </c>
-      <c r="E41" s="28" t="n">
+      <c r="E41" s="29" t="n">
         <v>1.13</v>
       </c>
     </row>
@@ -4056,7 +4054,7 @@
       <c r="D42" s="5" t="n">
         <v>0.95</v>
       </c>
-      <c r="E42" s="28" t="n">
+      <c r="E42" s="29" t="n">
         <v>1.43</v>
       </c>
     </row>
@@ -4079,7 +4077,7 @@
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B44" s="5" t="n">
         <v>0</v>
@@ -4096,7 +4094,7 @@
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B45" s="5" t="n">
         <v>0.25</v>
@@ -4113,7 +4111,7 @@
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B46" s="5" t="n">
         <v>0.3</v>
@@ -4130,7 +4128,7 @@
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B47" s="5" t="n">
         <v>0.35</v>
@@ -4147,7 +4145,7 @@
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B48" s="5" t="n">
         <v>0</v>
@@ -4164,7 +4162,7 @@
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B49" s="5" t="n">
         <v>0.06</v>
@@ -4181,7 +4179,7 @@
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B50" s="5" t="n">
         <v>0.07</v>
@@ -4198,7 +4196,7 @@
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B51" s="5" t="n">
         <v>0.085</v>
@@ -4215,7 +4213,7 @@
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B52" s="5" t="n">
         <v>0.1</v>
@@ -4402,7 +4400,7 @@
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B63" s="5" t="n">
         <v>0</v>
@@ -4419,7 +4417,7 @@
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B64" s="5" t="n">
         <v>0.6</v>
@@ -4430,13 +4428,13 @@
       <c r="D64" s="5" t="n">
         <v>0.5</v>
       </c>
-      <c r="E64" s="28" t="n">
+      <c r="E64" s="29" t="n">
         <v>0.5</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B65" s="5" t="n">
         <v>0.66</v>
@@ -4447,13 +4445,13 @@
       <c r="D65" s="5" t="n">
         <v>0.75</v>
       </c>
-      <c r="E65" s="28" t="n">
+      <c r="E65" s="29" t="n">
         <v>0.75</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B66" s="5" t="n">
         <v>0.7</v>
@@ -4464,13 +4462,13 @@
       <c r="D66" s="5" t="n">
         <v>0.95</v>
       </c>
-      <c r="E66" s="28" t="n">
+      <c r="E66" s="29" t="n">
         <v>0.95</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B67" s="5" t="n">
         <v>0.75</v>
@@ -4514,12 +4512,12 @@
   <dimension ref="A1:X65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A16" activeCellId="1" sqref="A38:A41 A16"/>
+      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.4939271255061"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.6032388663968"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="22" width="8.1417004048583"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.63967611336032"/>
@@ -4527,7 +4525,7 @@
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="22" width="8.1417004048583"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.9230769230769"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="20.0323886639676"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="4.39271255060729"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="22" width="8.1417004048583"/>
@@ -4725,7 +4723,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B7" s="5" t="n">
         <v>0</v>
@@ -4755,7 +4753,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B8" s="5" t="n">
         <v>0.6</v>
@@ -4785,7 +4783,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B9" s="5" t="n">
         <v>0.66</v>
@@ -4806,7 +4804,7 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B10" s="5" t="n">
         <v>0.7</v>
@@ -4827,7 +4825,7 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B11" s="5" t="n">
         <v>0.75</v>
@@ -4857,7 +4855,7 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B12" s="5" t="n">
         <v>0</v>
@@ -4887,7 +4885,7 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B13" s="5" t="n">
         <v>0.25</v>
@@ -4917,7 +4915,7 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B14" s="5" t="n">
         <v>0.3</v>
@@ -4947,7 +4945,7 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B15" s="5" t="n">
         <v>0.35</v>
@@ -5618,7 +5616,7 @@
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B39" s="5" t="n">
         <v>0</v>
@@ -5647,7 +5645,7 @@
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B40" s="5" t="n">
         <v>0.25</v>
@@ -5676,7 +5674,7 @@
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B41" s="5" t="n">
         <v>0.3</v>
@@ -5704,7 +5702,7 @@
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B42" s="5" t="n">
         <v>0.35</v>
@@ -5763,7 +5761,7 @@
       <c r="D44" s="5" t="n">
         <v>0.5</v>
       </c>
-      <c r="E44" s="28" t="n">
+      <c r="E44" s="29" t="n">
         <v>0.5</v>
       </c>
       <c r="G44" s="0"/>
@@ -5783,7 +5781,7 @@
       <c r="D45" s="5" t="n">
         <v>0.75</v>
       </c>
-      <c r="E45" s="28" t="n">
+      <c r="E45" s="29" t="n">
         <v>0.75</v>
       </c>
       <c r="G45" s="0"/>
@@ -5803,7 +5801,7 @@
       <c r="D46" s="5" t="n">
         <v>0.95</v>
       </c>
-      <c r="E46" s="28" t="n">
+      <c r="E46" s="29" t="n">
         <v>0.95</v>
       </c>
       <c r="G46" s="0"/>
@@ -5832,7 +5830,7 @@
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B48" s="5" t="n">
         <v>0</v>
@@ -5852,7 +5850,7 @@
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B49" s="5" t="n">
         <v>0.15</v>
@@ -5863,7 +5861,7 @@
       <c r="D49" s="5" t="n">
         <v>0.5</v>
       </c>
-      <c r="E49" s="28" t="n">
+      <c r="E49" s="29" t="n">
         <v>0.5</v>
       </c>
       <c r="G49" s="0"/>
@@ -5872,7 +5870,7 @@
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B50" s="5" t="n">
         <v>0.2</v>
@@ -5883,7 +5881,7 @@
       <c r="D50" s="5" t="n">
         <v>0.75</v>
       </c>
-      <c r="E50" s="28" t="n">
+      <c r="E50" s="29" t="n">
         <v>0.75</v>
       </c>
       <c r="G50" s="0"/>
@@ -5892,7 +5890,7 @@
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B51" s="5" t="n">
         <v>0.25</v>
@@ -5903,13 +5901,13 @@
       <c r="D51" s="5" t="n">
         <v>0.95</v>
       </c>
-      <c r="E51" s="28" t="n">
+      <c r="E51" s="29" t="n">
         <v>0.95</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B52" s="5" t="n">
         <v>0.3</v>
@@ -5926,7 +5924,7 @@
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B53" s="5" t="n">
         <v>0</v>
@@ -5943,7 +5941,7 @@
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B54" s="5" t="n">
         <v>0.25</v>
@@ -5960,7 +5958,7 @@
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B55" s="5" t="n">
         <v>0.3</v>
@@ -5977,7 +5975,7 @@
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B56" s="5" t="n">
         <v>0.35</v>
@@ -5994,7 +5992,7 @@
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B57" s="5" t="n">
         <v>0</v>
@@ -6011,7 +6009,7 @@
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B58" s="5" t="n">
         <v>0.2</v>
@@ -6028,7 +6026,7 @@
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B59" s="5" t="n">
         <v>0.3</v>
@@ -6045,7 +6043,7 @@
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B60" s="5" t="n">
         <v>0</v>
@@ -6062,7 +6060,7 @@
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B61" s="5" t="n">
         <v>0.6</v>
@@ -6079,7 +6077,7 @@
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B62" s="5" t="n">
         <v>0.66</v>
@@ -6096,7 +6094,7 @@
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B63" s="5" t="n">
         <v>0.7</v>
@@ -6113,7 +6111,7 @@
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B64" s="5" t="n">
         <v>0.75</v>
@@ -6243,7 +6241,7 @@
       <c r="D71" s="5" t="n">
         <v>0.5</v>
       </c>
-      <c r="E71" s="28" t="n">
+      <c r="E71" s="29" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -6260,7 +6258,7 @@
       <c r="D72" s="5" t="n">
         <v>0.75</v>
       </c>
-      <c r="E72" s="28" t="n">
+      <c r="E72" s="29" t="n">
         <v>0.75</v>
       </c>
     </row>
@@ -6277,7 +6275,7 @@
       <c r="D73" s="5" t="n">
         <v>0.95</v>
       </c>
-      <c r="E73" s="28" t="n">
+      <c r="E73" s="29" t="n">
         <v>0.95</v>
       </c>
     </row>
@@ -6300,7 +6298,7 @@
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B75" s="5" t="n">
         <v>0</v>
@@ -6317,7 +6315,7 @@
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B76" s="5" t="n">
         <v>0.2</v>
@@ -6334,7 +6332,7 @@
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B77" s="5" t="n">
         <v>0.3</v>
@@ -6377,12 +6375,12 @@
   <dimension ref="A1:N65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I49" activeCellId="1" sqref="A38:A41 I49"/>
+      <selection pane="topLeft" activeCell="I49" activeCellId="0" sqref="I49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.1376518218623"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.3522267206478"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.63967611336032"/>
@@ -6390,7 +6388,7 @@
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.3157894736842"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.4251012145749"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="4.39271255060729"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="7.49797570850202"/>
@@ -6527,7 +6525,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B7" s="5" t="n">
         <v>0</v>
@@ -6544,7 +6542,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B8" s="5" t="n">
         <v>0.6</v>
@@ -6561,7 +6559,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B9" s="5" t="n">
         <v>0.66</v>
@@ -6578,7 +6576,7 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B10" s="5" t="n">
         <v>0.7</v>
@@ -6595,7 +6593,7 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B11" s="5" t="n">
         <v>0.75</v>
@@ -6612,7 +6610,7 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B12" s="5" t="n">
         <v>0</v>
@@ -6629,7 +6627,7 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B13" s="5" t="n">
         <v>0.05</v>
@@ -6646,7 +6644,7 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B14" s="5" t="n">
         <v>0.15</v>
@@ -6663,7 +6661,7 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B15" s="5" t="n">
         <v>0</v>
@@ -6680,7 +6678,7 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B16" s="5" t="n">
         <v>0.3</v>
@@ -6697,7 +6695,7 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B17" s="5" t="n">
         <v>0.33</v>
@@ -6714,7 +6712,7 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B18" s="5" t="n">
         <v>0.35</v>
@@ -6738,7 +6736,7 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B19" s="5" t="n">
         <v>0.38</v>
@@ -6880,7 +6878,7 @@
       <c r="D26" s="5" t="n">
         <v>0.5</v>
       </c>
-      <c r="E26" s="28" t="n">
+      <c r="E26" s="29" t="n">
         <v>0.25</v>
       </c>
     </row>
@@ -6903,7 +6901,7 @@
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B28" s="5" t="n">
         <v>0</v>
@@ -6920,7 +6918,7 @@
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B29" s="5" t="n">
         <v>0.2</v>
@@ -6937,7 +6935,7 @@
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B30" s="5" t="n">
         <v>0.33</v>
@@ -7022,7 +7020,7 @@
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B35" s="5" t="n">
         <v>0</v>
@@ -7039,7 +7037,7 @@
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B36" s="5" t="n">
         <v>0.6</v>
@@ -7056,7 +7054,7 @@
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B37" s="5" t="n">
         <v>0.66</v>
@@ -7073,7 +7071,7 @@
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B38" s="5" t="n">
         <v>0.7</v>
@@ -7090,7 +7088,7 @@
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B39" s="5" t="n">
         <v>0.75</v>
@@ -7107,7 +7105,7 @@
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B40" s="5" t="n">
         <v>0</v>
@@ -7124,7 +7122,7 @@
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B41" s="5" t="n">
         <v>0.6</v>
@@ -7141,7 +7139,7 @@
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B42" s="5" t="n">
         <v>0.66</v>
@@ -7158,7 +7156,7 @@
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B43" s="5" t="n">
         <v>0.7</v>
@@ -7175,7 +7173,7 @@
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B44" s="5" t="n">
         <v>0.75</v>
@@ -7192,7 +7190,7 @@
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B45" s="5" t="n">
         <v>0</v>
@@ -7209,7 +7207,7 @@
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B46" s="5" t="n">
         <v>0.25</v>
@@ -7226,7 +7224,7 @@
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B47" s="5" t="n">
         <v>0.3</v>
@@ -7243,7 +7241,7 @@
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B48" s="5" t="n">
         <v>0.35</v>
@@ -7286,19 +7284,19 @@
   <dimension ref="A1:E42"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E42" activeCellId="1" sqref="A38:A41 E42"/>
+      <selection pane="topLeft" activeCell="E42" activeCellId="0" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.995951417004"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="19.3886639676113"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.1012145748988"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="19.4939271255061"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.3562753036437"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.1417004048583"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.9230769230769"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="20.0323886639676"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="4.39271255060729"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.1417004048583"/>
@@ -8019,12 +8017,12 @@
   <dimension ref="A1:O18"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E18" activeCellId="1" sqref="A38:A41 E18"/>
+      <selection pane="topLeft" activeCell="E18" activeCellId="0" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="35.1336032388664"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="35.3481781376518"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="13.9271255060729"/>
@@ -8032,7 +8030,7 @@
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.9230769230769"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="20.0323886639676"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="4.39271255060729"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="7.49797570850202"/>
@@ -8343,20 +8341,20 @@
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E18" activeCellId="1" sqref="A38:A41 E18"/>
+      <selection pane="topLeft" activeCell="E18" activeCellId="0" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.2105263157895"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.5668016194332"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.3157894736842"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.6761133603239"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="12.748987854251"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="12.8542510121458"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.9230769230769"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="20.0323886639676"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="4.39271255060729"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="7.49797570850202"/>
@@ -8666,27 +8664,27 @@
   <dimension ref="A1:S32"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E32" activeCellId="1" sqref="A38:A41 E32"/>
+      <selection pane="topLeft" activeCell="E32" activeCellId="0" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.0647773279352"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.1012145748988"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.4615384615385"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.3846153846154"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.2105263157895"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.5668016194332"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="14.0323886639676"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.7813765182186"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.9230769230769"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="20.0323886639676"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="4.39271255060729"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.1417004048583"/>
     <col collapsed="false" hidden="false" max="13" min="13" style="0" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="0" width="6.63967611336032"/>
     <col collapsed="false" hidden="false" max="18" min="15" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="13.2834008097166"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -9227,12 +9225,12 @@
   <dimension ref="A1:S32"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E32" activeCellId="1" sqref="A38:A41 E32"/>
+      <selection pane="topLeft" activeCell="E32" activeCellId="0" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="55.4858299595142"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="55.914979757085"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.46153846153846"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.78542510121457"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="18" width="6.63967611336032"/>
@@ -9240,14 +9238,14 @@
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.9230769230769"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="20.0323886639676"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="4.39271255060729"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.1417004048583"/>
     <col collapsed="false" hidden="false" max="13" min="13" style="0" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="0" width="6.63967611336032"/>
     <col collapsed="false" hidden="false" max="18" min="15" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="13.2834008097166"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -9795,12 +9793,12 @@
   <dimension ref="A1:S65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E29" activeCellId="1" sqref="A38:A41 E29"/>
+      <selection pane="topLeft" activeCell="E29" activeCellId="0" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.7044534412955"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.919028340081"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.1417004048583"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.3886639676113"/>
@@ -9808,7 +9806,7 @@
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.1417004048583"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.9230769230769"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="20.0323886639676"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="4.39271255060729"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="7.49797570850202"/>
@@ -10332,12 +10330,12 @@
   <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E29" activeCellId="1" sqref="A38:A41 E29"/>
+      <selection pane="topLeft" activeCell="E29" activeCellId="0" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.4210526315789"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.7408906882591"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.1417004048583"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.67611336032389"/>
@@ -10345,7 +10343,7 @@
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.1417004048583"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.9230769230769"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="20.0323886639676"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="4.39271255060729"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="7.49797570850202"/>
@@ -10831,13 +10829,13 @@
   </sheetPr>
   <dimension ref="A1:S65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A38" activeCellId="0" sqref="A38:A41"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A19" activeCellId="0" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.1012145748988"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.4210526315789"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="22" width="8.1417004048583"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="10" width="6.63967611336032"/>
@@ -10845,7 +10843,7 @@
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="22" width="8.1417004048583"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="10" width="19.9230769230769"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="10" width="20.0323886639676"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="4.39271255060729"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="22" width="8.1417004048583"/>
@@ -11407,8 +11405,8 @@
       <c r="S22" s="9"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
-        <v>20</v>
+      <c r="A23" s="25" t="s">
+        <v>7</v>
       </c>
       <c r="B23" s="5" t="n">
         <v>0</v>
@@ -11435,8 +11433,8 @@
       <c r="S23" s="9"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
-        <v>20</v>
+      <c r="A24" s="25" t="s">
+        <v>7</v>
       </c>
       <c r="B24" s="5" t="n">
         <v>0.6</v>
@@ -11462,8 +11460,8 @@
       <c r="S24" s="16"/>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
-        <v>20</v>
+      <c r="A25" s="25" t="s">
+        <v>7</v>
       </c>
       <c r="B25" s="5" t="n">
         <v>0.66</v>
@@ -11489,8 +11487,8 @@
       <c r="S25" s="16"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
-        <v>20</v>
+      <c r="A26" s="25" t="s">
+        <v>7</v>
       </c>
       <c r="B26" s="5" t="n">
         <v>0.7</v>
@@ -11516,8 +11514,8 @@
       <c r="S26" s="16"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
-        <v>20</v>
+      <c r="A27" s="25" t="s">
+        <v>7</v>
       </c>
       <c r="B27" s="5" t="n">
         <v>0.75</v>
@@ -11544,7 +11542,7 @@
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B28" s="5" t="n">
         <v>0</v>
@@ -11571,7 +11569,7 @@
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B29" s="5" t="n">
         <v>0.3</v>
@@ -11598,7 +11596,7 @@
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B30" s="5" t="n">
         <v>0.35</v>
@@ -11622,7 +11620,7 @@
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B31" s="5" t="n">
         <v>0.4</v>
@@ -11645,7 +11643,7 @@
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B32" s="5" t="n">
         <v>0</v>
@@ -11669,7 +11667,7 @@
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B33" s="5" t="n">
         <v>0.6</v>
@@ -11692,7 +11690,7 @@
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B34" s="5" t="n">
         <v>0.66</v>
@@ -11715,7 +11713,7 @@
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B35" s="5" t="n">
         <v>0.7</v>
@@ -11738,7 +11736,7 @@
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B36" s="5" t="n">
         <v>0.75</v>
@@ -11798,6 +11796,12 @@
       <c r="E38" s="9" t="n">
         <v>1.5</v>
       </c>
+      <c r="G38" s="0"/>
+      <c r="I38" s="0"/>
+      <c r="L38" s="0"/>
+      <c r="N38" s="0"/>
+      <c r="Q38" s="0"/>
+      <c r="S38" s="0"/>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="7" t="s">
@@ -11815,6 +11819,12 @@
       <c r="E39" s="9" t="n">
         <v>2.3</v>
       </c>
+      <c r="G39" s="0"/>
+      <c r="I39" s="0"/>
+      <c r="L39" s="0"/>
+      <c r="N39" s="0"/>
+      <c r="Q39" s="0"/>
+      <c r="S39" s="0"/>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="7" t="s">
@@ -11832,6 +11842,12 @@
       <c r="E40" s="9" t="n">
         <v>2.9</v>
       </c>
+      <c r="G40" s="0"/>
+      <c r="I40" s="0"/>
+      <c r="L40" s="0"/>
+      <c r="N40" s="0"/>
+      <c r="Q40" s="0"/>
+      <c r="S40" s="0"/>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="7" t="s">
@@ -11849,6 +11865,12 @@
       <c r="E41" s="10" t="n">
         <v>3</v>
       </c>
+      <c r="G41" s="0"/>
+      <c r="I41" s="0"/>
+      <c r="L41" s="0"/>
+      <c r="N41" s="0"/>
+      <c r="Q41" s="0"/>
+      <c r="S41" s="0"/>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
@@ -11866,6 +11888,12 @@
       <c r="E42" s="9" t="n">
         <v>0</v>
       </c>
+      <c r="G42" s="0"/>
+      <c r="I42" s="0"/>
+      <c r="L42" s="0"/>
+      <c r="N42" s="0"/>
+      <c r="Q42" s="0"/>
+      <c r="S42" s="0"/>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
@@ -11883,6 +11911,12 @@
       <c r="E43" s="9" t="n">
         <v>0.5</v>
       </c>
+      <c r="G43" s="0"/>
+      <c r="I43" s="0"/>
+      <c r="L43" s="0"/>
+      <c r="N43" s="0"/>
+      <c r="Q43" s="0"/>
+      <c r="S43" s="0"/>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
@@ -11900,10 +11934,16 @@
       <c r="E44" s="9" t="n">
         <v>1</v>
       </c>
+      <c r="G44" s="0"/>
+      <c r="I44" s="0"/>
+      <c r="L44" s="0"/>
+      <c r="N44" s="0"/>
+      <c r="Q44" s="0"/>
+      <c r="S44" s="0"/>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B45" s="5" t="n">
         <v>0</v>
@@ -11917,10 +11957,16 @@
       <c r="E45" s="9" t="n">
         <v>0</v>
       </c>
+      <c r="G45" s="0"/>
+      <c r="I45" s="0"/>
+      <c r="L45" s="0"/>
+      <c r="N45" s="0"/>
+      <c r="Q45" s="0"/>
+      <c r="S45" s="0"/>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B46" s="5" t="n">
         <v>0.06</v>
@@ -11934,10 +11980,16 @@
       <c r="E46" s="9" t="n">
         <v>1.5</v>
       </c>
+      <c r="G46" s="0"/>
+      <c r="I46" s="0"/>
+      <c r="L46" s="0"/>
+      <c r="N46" s="0"/>
+      <c r="Q46" s="0"/>
+      <c r="S46" s="0"/>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B47" s="5" t="n">
         <v>0.07</v>
@@ -11951,10 +12003,16 @@
       <c r="E47" s="9" t="n">
         <v>2.3</v>
       </c>
+      <c r="G47" s="0"/>
+      <c r="I47" s="0"/>
+      <c r="L47" s="0"/>
+      <c r="N47" s="0"/>
+      <c r="Q47" s="0"/>
+      <c r="S47" s="0"/>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B48" s="5" t="n">
         <v>0.085</v>
@@ -11968,10 +12026,16 @@
       <c r="E48" s="9" t="n">
         <v>2.9</v>
       </c>
+      <c r="G48" s="0"/>
+      <c r="I48" s="0"/>
+      <c r="L48" s="0"/>
+      <c r="N48" s="0"/>
+      <c r="Q48" s="0"/>
+      <c r="S48" s="0"/>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B49" s="5" t="n">
         <v>0.1</v>
@@ -11985,6 +12049,12 @@
       <c r="E49" s="10" t="n">
         <v>3</v>
       </c>
+      <c r="G49" s="0"/>
+      <c r="I49" s="0"/>
+      <c r="L49" s="0"/>
+      <c r="N49" s="0"/>
+      <c r="Q49" s="0"/>
+      <c r="S49" s="0"/>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
@@ -12002,6 +12072,12 @@
       <c r="E50" s="9" t="n">
         <v>0</v>
       </c>
+      <c r="G50" s="0"/>
+      <c r="I50" s="0"/>
+      <c r="L50" s="0"/>
+      <c r="N50" s="0"/>
+      <c r="Q50" s="0"/>
+      <c r="S50" s="0"/>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
@@ -12019,6 +12095,12 @@
       <c r="E51" s="9" t="n">
         <v>1.8</v>
       </c>
+      <c r="G51" s="0"/>
+      <c r="I51" s="0"/>
+      <c r="L51" s="0"/>
+      <c r="N51" s="0"/>
+      <c r="Q51" s="0"/>
+      <c r="S51" s="0"/>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
@@ -12036,6 +12118,12 @@
       <c r="E52" s="9" t="n">
         <v>2.6</v>
       </c>
+      <c r="G52" s="0"/>
+      <c r="I52" s="0"/>
+      <c r="L52" s="0"/>
+      <c r="N52" s="0"/>
+      <c r="Q52" s="0"/>
+      <c r="S52" s="0"/>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
@@ -12053,6 +12141,12 @@
       <c r="E53" s="9" t="n">
         <v>0.9</v>
       </c>
+      <c r="G53" s="0"/>
+      <c r="I53" s="0"/>
+      <c r="L53" s="0"/>
+      <c r="N53" s="0"/>
+      <c r="Q53" s="0"/>
+      <c r="S53" s="0"/>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
@@ -12070,10 +12164,16 @@
       <c r="E54" s="17" t="n">
         <v>3.5</v>
       </c>
+      <c r="G54" s="0"/>
+      <c r="I54" s="0"/>
+      <c r="L54" s="0"/>
+      <c r="N54" s="0"/>
+      <c r="Q54" s="0"/>
+      <c r="S54" s="0"/>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="0" t="s">
-        <v>24</v>
+      <c r="A55" s="25" t="s">
+        <v>8</v>
       </c>
       <c r="B55" s="5" t="n">
         <v>0</v>
@@ -12087,10 +12187,16 @@
       <c r="E55" s="9" t="n">
         <v>0</v>
       </c>
+      <c r="G55" s="0"/>
+      <c r="I55" s="0"/>
+      <c r="L55" s="0"/>
+      <c r="N55" s="0"/>
+      <c r="Q55" s="0"/>
+      <c r="S55" s="0"/>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="0" t="s">
-        <v>24</v>
+      <c r="A56" s="25" t="s">
+        <v>8</v>
       </c>
       <c r="B56" s="5" t="n">
         <v>0.3</v>
@@ -12104,10 +12210,16 @@
       <c r="E56" s="9" t="n">
         <v>0.8</v>
       </c>
+      <c r="G56" s="0"/>
+      <c r="I56" s="0"/>
+      <c r="L56" s="0"/>
+      <c r="N56" s="0"/>
+      <c r="Q56" s="0"/>
+      <c r="S56" s="0"/>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="0" t="s">
-        <v>24</v>
+      <c r="A57" s="25" t="s">
+        <v>8</v>
       </c>
       <c r="B57" s="5" t="n">
         <v>0.35</v>
@@ -12121,10 +12233,16 @@
       <c r="E57" s="9" t="n">
         <v>1.1</v>
       </c>
+      <c r="G57" s="0"/>
+      <c r="I57" s="0"/>
+      <c r="L57" s="0"/>
+      <c r="N57" s="0"/>
+      <c r="Q57" s="0"/>
+      <c r="S57" s="0"/>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="0" t="s">
-        <v>24</v>
+      <c r="A58" s="25" t="s">
+        <v>8</v>
       </c>
       <c r="B58" s="5" t="n">
         <v>0.4</v>
@@ -12138,10 +12256,16 @@
       <c r="E58" s="9" t="n">
         <v>1.4</v>
       </c>
+      <c r="G58" s="0"/>
+      <c r="I58" s="0"/>
+      <c r="L58" s="0"/>
+      <c r="N58" s="0"/>
+      <c r="Q58" s="0"/>
+      <c r="S58" s="0"/>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="0" t="s">
-        <v>24</v>
+      <c r="A59" s="25" t="s">
+        <v>8</v>
       </c>
       <c r="B59" s="5" t="n">
         <v>0.45</v>
@@ -12155,6 +12279,42 @@
       <c r="E59" s="16" t="n">
         <v>1.5</v>
       </c>
+      <c r="G59" s="0"/>
+      <c r="I59" s="0"/>
+      <c r="L59" s="0"/>
+      <c r="N59" s="0"/>
+      <c r="Q59" s="0"/>
+      <c r="S59" s="0"/>
+    </row>
+    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B60" s="0"/>
+      <c r="D60" s="0"/>
+      <c r="G60" s="0"/>
+      <c r="I60" s="0"/>
+      <c r="L60" s="0"/>
+      <c r="N60" s="0"/>
+      <c r="Q60" s="0"/>
+      <c r="S60" s="0"/>
+    </row>
+    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B61" s="0"/>
+      <c r="D61" s="0"/>
+      <c r="G61" s="0"/>
+      <c r="I61" s="0"/>
+      <c r="L61" s="0"/>
+      <c r="N61" s="0"/>
+      <c r="Q61" s="0"/>
+      <c r="S61" s="0"/>
+    </row>
+    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B62" s="0"/>
+      <c r="D62" s="0"/>
+      <c r="G62" s="0"/>
+      <c r="I62" s="0"/>
+      <c r="L62" s="0"/>
+      <c r="N62" s="0"/>
+      <c r="Q62" s="0"/>
+      <c r="S62" s="0"/>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B63" s="0"/>

</xml_diff>